<commit_message>
Fixed to allow counting of infinite entries
</commit_message>
<xml_diff>
--- a/Graph.xlsx
+++ b/Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\futeb\anime-list-to-csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alt\MyAnimeListToCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{EF630CCF-6D5B-42E1-B0AA-1BCF358780A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EB87F9-F18C-43E7-B8AC-9619741D7283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="15600"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="out (2)" sheetId="3" r:id="rId1"/>
@@ -38,11 +38,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - out" description="Ligação à consulta 'out' no livro." type="5" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - out" description="Ligação à consulta 'out' no livro." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=out;Extended Properties=&quot;&quot;" command="SELECT * FROM [out]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Consulta - out (2)" description="Ligação à consulta 'out (2)' no livro." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Consulta - out (2)" description="Ligação à consulta 'out (2)' no livro." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;out (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [out (2)]"/>
   </connection>
 </connections>
@@ -732,7 +732,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3833,7 +3833,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DadosExternos_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_2" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="10">
     <queryTableFields count="9">
       <queryTableField id="1" name="Name" tableColumnId="1"/>
@@ -3851,21 +3851,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="out__2" displayName="out__2" ref="A1:I91" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:I91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="out__2" displayName="out__2" ref="A1:I91" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I91" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I91">
     <sortCondition ref="H1:H91"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" uniqueName="2" name="Status" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" uniqueName="3" name="Score" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name="Eps watched" queryTableFieldId="4"/>
-    <tableColumn id="5" uniqueName="5" name="Start date" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" uniqueName="6" name="Finish date" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="7" uniqueName="7" name="Season" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="8" uniqueName="8" name="Year" queryTableFieldId="8"/>
-    <tableColumn id="9" uniqueName="9" name="Genres" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Status" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Score" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Eps watched" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Start date" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Finish date" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Season" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Year" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Genres" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4167,31 +4167,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V60" sqref="V60"/>
+    <sheetView tabSelected="1" topLeftCell="H41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="81.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1796875" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
     <col min="17" max="17" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>101</v>
       </c>
@@ -4266,11 +4266,11 @@
         <v>171</v>
       </c>
       <c r="N2">
-        <f>COUNTIFS($G$2:$G$91,$M2,$B$2:$B$91,N$1)</f>
+        <f>COUNTIFS($G:$G,$M2,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:R2" si="0">COUNTIFS($G$2:$G$91,$M2,$B$2:$B$91,O$1)</f>
+        <f t="shared" ref="O2:R2" si="0">COUNTIFS($G:$G,$M2,$B:$B,O$1)</f>
         <v>0</v>
       </c>
       <c r="P2">
@@ -4286,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>127</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:R65" si="1">COUNTIFS($G$2:$G$91,$M3,$B$2:$B$91,N$1)</f>
+        <f t="shared" ref="N3:R65" si="1">COUNTIFS($G:$G,$M3,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O3">
@@ -4333,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>126</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>123</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>114</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>148</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>147</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>90</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>105</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>109</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>133</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>144</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>85</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>117</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>122</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>107</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>125</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>142</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>92</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>129</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>119</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>100</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>118</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>140</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>83</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>0</v>
       </c>
       <c r="O51">
-        <f t="shared" ref="O51:R65" si="2">COUNTIFS($G$2:$G$91,$M51,$B$2:$B$91,O$1)</f>
+        <f t="shared" ref="O51:R65" si="2">COUNTIFS($G:$G,$M51,$B:$B,O$1)</f>
         <v>0</v>
       </c>
       <c r="P51">
@@ -6621,7 +6621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>79</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>98</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>116</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>31</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>131</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>95</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>141</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>13</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>34</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>37</v>
       </c>
@@ -7292,7 +7292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>121</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>146</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>69</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>20</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>36</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>43</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>63</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>27</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>68</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>89</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>80</v>
       </c>
@@ -7616,7 +7616,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>81</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>82</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>128</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>132</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>106</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>120</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>15</v>
       </c>
@@ -7800,7 +7800,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>18</v>
       </c>
@@ -7824,7 +7824,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>19</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>111</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>135</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>137</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>139</v>
       </c>
@@ -7940,12 +7940,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor fix on Excel sheet
</commit_message>
<xml_diff>
--- a/Graph.xlsx
+++ b/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\futeb\anime-list-to-csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E283C385-6CA9-4689-8C7C-27CD7D3182DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86649955-D169-4496-A33B-79109EDC1D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="229">
   <si>
     <t>Name</t>
   </si>
@@ -749,6 +749,12 @@
   </si>
   <si>
     <t>Import your data, then copy it to the "Analysis" sheet!</t>
+  </si>
+  <si>
+    <t>Summer 2022</t>
+  </si>
+  <si>
+    <t>Fall 2022</t>
   </si>
 </sst>
 </file>
@@ -806,6 +812,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -828,9 +837,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -963,9 +969,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$M$2:$M$65</c:f>
+              <c:f>Analysis!$M$2:$M$69</c:f>
               <c:strCache>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>Winter 2006</c:v>
                 </c:pt>
@@ -1157,16 +1163,28 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>Fall 2021</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Winter 2022</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Spring 2022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Summer 2022</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Fall 2022</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$Q$2:$Q$65</c:f>
+              <c:f>Analysis!$Q$2:$Q$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1358,6 +1376,18 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,9 +1424,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$M$2:$M$65</c:f>
+              <c:f>Analysis!$M$2:$M$69</c:f>
               <c:strCache>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>Winter 2006</c:v>
                 </c:pt>
@@ -1588,16 +1618,28 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>Fall 2021</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Winter 2022</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Spring 2022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Summer 2022</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Fall 2022</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$O$2:$O$65</c:f>
+              <c:f>Analysis!$O$2:$O$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1788,6 +1830,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1825,9 +1879,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$M$2:$M$65</c:f>
+              <c:f>Analysis!$M$2:$M$69</c:f>
               <c:strCache>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>Winter 2006</c:v>
                 </c:pt>
@@ -2019,16 +2073,28 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>Fall 2021</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Winter 2022</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Spring 2022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Summer 2022</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Fall 2022</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$P$2:$P$65</c:f>
+              <c:f>Analysis!$P$2:$P$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2220,6 +2286,18 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2256,9 +2334,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$M$2:$M$65</c:f>
+              <c:f>Analysis!$M$2:$M$69</c:f>
               <c:strCache>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>Winter 2006</c:v>
                 </c:pt>
@@ -2450,16 +2528,28 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>Fall 2021</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Winter 2022</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Spring 2022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Summer 2022</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Fall 2022</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$R$2:$R$65</c:f>
+              <c:f>Analysis!$R$2:$R$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2651,6 +2741,18 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2687,9 +2789,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$M$2:$M$65</c:f>
+              <c:f>Analysis!$M$2:$M$69</c:f>
               <c:strCache>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>Winter 2006</c:v>
                 </c:pt>
@@ -2881,16 +2983,28 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>Fall 2021</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Winter 2022</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Spring 2022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Summer 2022</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Fall 2022</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$N$2:$N$65</c:f>
+              <c:f>Analysis!$N$2:$N$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="64"/>
+                <c:ptCount val="68"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3082,6 +3196,18 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3330,7 +3456,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-PT"/>
-              <a:t>Anime watched per season</a:t>
+              <a:t>Anime watched per year</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5428,16 +5554,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1471612</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5464,16 +5590,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1457325</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>14288</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>185739</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>452438</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>138114</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5543,15 +5669,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{03BD9E12-F1C3-401A-A934-06164C29B91C}" name="out__7" displayName="out__7" ref="A1:I91" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I91" xr:uid="{03BD9E12-F1C3-401A-A934-06164C29B91C}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{96082CFC-DF56-4F49-9837-07C2F8732101}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{501C03C7-78A5-4A0C-9315-9658FE5E5720}" uniqueName="2" name="Status" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{96082CFC-DF56-4F49-9837-07C2F8732101}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{501C03C7-78A5-4A0C-9315-9658FE5E5720}" uniqueName="2" name="Status" queryTableFieldId="2" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{17DD36EE-25D6-431C-AD32-FCD47D6E4730}" uniqueName="3" name="Score" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{513C9B46-14B1-4260-83B0-394DEB921200}" uniqueName="4" name="Eps watched" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{0E88CD67-6F4D-4DEB-BD9B-FF0B340C336D}" uniqueName="5" name="Start date" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{4CE32D1B-4D6A-4F52-8618-846470A5A9E3}" uniqueName="6" name="Finish date" queryTableFieldId="6" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{37EA1B4E-1C2B-4A31-835C-23BF15DE95AB}" uniqueName="7" name="Season" queryTableFieldId="7" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{0E88CD67-6F4D-4DEB-BD9B-FF0B340C336D}" uniqueName="5" name="Start date" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4CE32D1B-4D6A-4F52-8618-846470A5A9E3}" uniqueName="6" name="Finish date" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{37EA1B4E-1C2B-4A31-835C-23BF15DE95AB}" uniqueName="7" name="Season" queryTableFieldId="7" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{5AFDD098-F316-4E65-84D3-405E3082D177}" uniqueName="8" name="Year" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{C1082522-91C8-4E27-99BC-DE1DD566EA94}" uniqueName="9" name="Genres" queryTableFieldId="9" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{C1082522-91C8-4E27-99BC-DE1DD566EA94}" uniqueName="9" name="Genres" queryTableFieldId="9" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5565,14 +5691,14 @@
     <sortCondition descending="1" ref="G2:G91" customList="Winter,Spring,Summer,Fall"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Status" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Status" queryTableFieldId="2" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Score" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Eps watched" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Start date" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Finish date" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Season" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Year" queryTableFieldId="8" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Start date" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Finish date" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Season" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Year" queryTableFieldId="8" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Genres" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6658,8 +6784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="J35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI87" sqref="AI87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6775,23 +6901,23 @@
         <v>171</v>
       </c>
       <c r="N2">
-        <f>COUNTIFS($G:$G,$M2,$B:$B,N$1)</f>
+        <f t="shared" ref="N2:R11" si="0">COUNTIFS($G:$G,$M2,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O2">
-        <f>COUNTIFS($G:$G,$M2,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>COUNTIFS($G:$G,$M2,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>COUNTIFS($G:$G,$M2,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R2">
-        <f>COUNTIFS($G:$G,$M2,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T2">
@@ -6802,19 +6928,19 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <f t="shared" ref="V2:Y2" si="0">COUNTIFS($H:$H,$T2,$B:$B,V$1)</f>
+        <f t="shared" ref="V2:Y2" si="1">COUNTIFS($H:$H,$T2,$B:$B,V$1)</f>
         <v>0</v>
       </c>
       <c r="W2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="X2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6845,46 +6971,46 @@
         <v>127</v>
       </c>
       <c r="N3">
-        <f>COUNTIFS($G:$G,$M3,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O3">
-        <f>COUNTIFS($G:$G,$M3,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P3">
-        <f>COUNTIFS($G:$G,$M3,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>COUNTIFS($G:$G,$M3,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R3">
-        <f>COUNTIFS($G:$G,$M3,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T3">
         <v>2007</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:Y18" si="1">COUNTIFS($H:$H,$T3,$B:$B,U$1)</f>
+        <f t="shared" ref="U3:Y18" si="2">COUNTIFS($H:$H,$T3,$B:$B,U$1)</f>
         <v>1</v>
       </c>
       <c r="V3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6915,46 +7041,46 @@
         <v>124</v>
       </c>
       <c r="N4">
-        <f>COUNTIFS($G:$G,$M4,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>COUNTIFS($G:$G,$M4,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f>COUNTIFS($G:$G,$M4,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f>COUNTIFS($G:$G,$M4,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R4">
-        <f>COUNTIFS($G:$G,$M4,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T4">
         <v>2008</v>
       </c>
       <c r="U4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6985,46 +7111,46 @@
         <v>73</v>
       </c>
       <c r="N5">
-        <f>COUNTIFS($G:$G,$M5,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5">
-        <f>COUNTIFS($G:$G,$M5,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P5">
-        <f>COUNTIFS($G:$G,$M5,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q5">
-        <f>COUNTIFS($G:$G,$M5,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R5">
-        <f>COUNTIFS($G:$G,$M5,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T5">
         <v>2009</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7055,46 +7181,46 @@
         <v>172</v>
       </c>
       <c r="N6">
-        <f>COUNTIFS($G:$G,$M6,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O6">
-        <f>COUNTIFS($G:$G,$M6,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P6">
-        <f>COUNTIFS($G:$G,$M6,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f>COUNTIFS($G:$G,$M6,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R6">
-        <f>COUNTIFS($G:$G,$M6,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T6">
         <v>2010</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="X6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7125,46 +7251,46 @@
         <v>48</v>
       </c>
       <c r="N7">
-        <f>COUNTIFS($G:$G,$M7,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O7">
-        <f>COUNTIFS($G:$G,$M7,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P7">
-        <f>COUNTIFS($G:$G,$M7,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>COUNTIFS($G:$G,$M7,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R7">
-        <f>COUNTIFS($G:$G,$M7,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T7">
         <v>2011</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7195,46 +7321,46 @@
         <v>150</v>
       </c>
       <c r="N8">
-        <f>COUNTIFS($G:$G,$M8,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O8">
-        <f>COUNTIFS($G:$G,$M8,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>COUNTIFS($G:$G,$M8,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f>COUNTIFS($G:$G,$M8,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R8">
-        <f>COUNTIFS($G:$G,$M8,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T8">
         <v>2012</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="W8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -7270,46 +7396,46 @@
         <v>151</v>
       </c>
       <c r="N9">
-        <f>COUNTIFS($G:$G,$M9,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O9">
-        <f>COUNTIFS($G:$G,$M9,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P9">
-        <f>COUNTIFS($G:$G,$M9,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f>COUNTIFS($G:$G,$M9,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R9">
-        <f>COUNTIFS($G:$G,$M9,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T9">
         <v>2013</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7345,46 +7471,46 @@
         <v>152</v>
       </c>
       <c r="N10">
-        <f>COUNTIFS($G:$G,$M10,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>COUNTIFS($G:$G,$M10,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P10">
-        <f>COUNTIFS($G:$G,$M10,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f>COUNTIFS($G:$G,$M10,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R10">
-        <f>COUNTIFS($G:$G,$M10,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T10">
         <v>2014</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7420,46 +7546,46 @@
         <v>153</v>
       </c>
       <c r="N11">
-        <f>COUNTIFS($G:$G,$M11,$B:$B,N$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>COUNTIFS($G:$G,$M11,$B:$B,O$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P11">
-        <f>COUNTIFS($G:$G,$M11,$B:$B,P$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f>COUNTIFS($G:$G,$M11,$B:$B,Q$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R11">
-        <f>COUNTIFS($G:$G,$M11,$B:$B,R$1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T11">
         <v>2015</v>
       </c>
       <c r="U11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7495,46 +7621,46 @@
         <v>154</v>
       </c>
       <c r="N12">
-        <f>COUNTIFS($G:$G,$M12,$B:$B,N$1)</f>
+        <f t="shared" ref="N12:R21" si="3">COUNTIFS($G:$G,$M12,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O12">
-        <f>COUNTIFS($G:$G,$M12,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P12">
-        <f>COUNTIFS($G:$G,$M12,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f>COUNTIFS($G:$G,$M12,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R12">
-        <f>COUNTIFS($G:$G,$M12,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T12">
         <v>2016</v>
       </c>
       <c r="U12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -7570,46 +7696,46 @@
         <v>65</v>
       </c>
       <c r="N13">
-        <f>COUNTIFS($G:$G,$M13,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O13">
-        <f>COUNTIFS($G:$G,$M13,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P13">
-        <f>COUNTIFS($G:$G,$M13,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f>COUNTIFS($G:$G,$M13,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R13">
-        <f>COUNTIFS($G:$G,$M13,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T13">
         <v>2017</v>
       </c>
       <c r="U13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7645,46 +7771,46 @@
         <v>155</v>
       </c>
       <c r="N14">
-        <f>COUNTIFS($G:$G,$M14,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>COUNTIFS($G:$G,$M14,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>COUNTIFS($G:$G,$M14,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>COUNTIFS($G:$G,$M14,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f>COUNTIFS($G:$G,$M14,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T14">
         <v>2018</v>
       </c>
       <c r="U14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="X14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7720,46 +7846,46 @@
         <v>30</v>
       </c>
       <c r="N15">
-        <f>COUNTIFS($G:$G,$M15,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O15">
-        <f>COUNTIFS($G:$G,$M15,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f>COUNTIFS($G:$G,$M15,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f>COUNTIFS($G:$G,$M15,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f>COUNTIFS($G:$G,$M15,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T15">
         <v>2019</v>
       </c>
       <c r="U15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="V15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -7795,46 +7921,46 @@
         <v>156</v>
       </c>
       <c r="N16">
-        <f>COUNTIFS($G:$G,$M16,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O16">
-        <f>COUNTIFS($G:$G,$M16,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P16">
-        <f>COUNTIFS($G:$G,$M16,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f>COUNTIFS($G:$G,$M16,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R16">
-        <f>COUNTIFS($G:$G,$M16,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T16">
         <v>2020</v>
       </c>
       <c r="U16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="V16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -7870,46 +7996,46 @@
         <v>115</v>
       </c>
       <c r="N17">
-        <f>COUNTIFS($G:$G,$M17,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O17">
-        <f>COUNTIFS($G:$G,$M17,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P17">
-        <f>COUNTIFS($G:$G,$M17,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q17">
-        <f>COUNTIFS($G:$G,$M17,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R17">
-        <f>COUNTIFS($G:$G,$M17,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T17">
         <v>2021</v>
       </c>
       <c r="U17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="V17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="W17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="X17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -7945,46 +8071,46 @@
         <v>157</v>
       </c>
       <c r="N18">
-        <f>COUNTIFS($G:$G,$M18,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O18">
-        <f>COUNTIFS($G:$G,$M18,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P18">
-        <f>COUNTIFS($G:$G,$M18,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q18">
-        <f>COUNTIFS($G:$G,$M18,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R18">
-        <f>COUNTIFS($G:$G,$M18,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T18">
         <v>2022</v>
       </c>
       <c r="U18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -8020,23 +8146,23 @@
         <v>75</v>
       </c>
       <c r="N19">
-        <f>COUNTIFS($G:$G,$M19,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O19">
-        <f>COUNTIFS($G:$G,$M19,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P19">
-        <f>COUNTIFS($G:$G,$M19,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q19">
-        <f>COUNTIFS($G:$G,$M19,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R19">
-        <f>COUNTIFS($G:$G,$M19,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -8072,23 +8198,23 @@
         <v>158</v>
       </c>
       <c r="N20">
-        <f>COUNTIFS($G:$G,$M20,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O20">
-        <f>COUNTIFS($G:$G,$M20,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P20">
-        <f>COUNTIFS($G:$G,$M20,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>COUNTIFS($G:$G,$M20,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R20">
-        <f>COUNTIFS($G:$G,$M20,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -8124,23 +8250,23 @@
         <v>149</v>
       </c>
       <c r="N21">
-        <f>COUNTIFS($G:$G,$M21,$B:$B,N$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O21">
-        <f>COUNTIFS($G:$G,$M21,$B:$B,O$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P21">
-        <f>COUNTIFS($G:$G,$M21,$B:$B,P$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q21">
-        <f>COUNTIFS($G:$G,$M21,$B:$B,Q$1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R21">
-        <f>COUNTIFS($G:$G,$M21,$B:$B,R$1)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -8176,23 +8302,23 @@
         <v>159</v>
       </c>
       <c r="N22">
-        <f>COUNTIFS($G:$G,$M22,$B:$B,N$1)</f>
+        <f t="shared" ref="N22:R31" si="4">COUNTIFS($G:$G,$M22,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O22">
-        <f>COUNTIFS($G:$G,$M22,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P22">
-        <f>COUNTIFS($G:$G,$M22,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q22">
-        <f>COUNTIFS($G:$G,$M22,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R22">
-        <f>COUNTIFS($G:$G,$M22,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8228,23 +8354,23 @@
         <v>91</v>
       </c>
       <c r="N23">
-        <f>COUNTIFS($G:$G,$M23,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O23">
-        <f>COUNTIFS($G:$G,$M23,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P23">
-        <f>COUNTIFS($G:$G,$M23,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q23">
-        <f>COUNTIFS($G:$G,$M23,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R23">
-        <f>COUNTIFS($G:$G,$M23,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8280,23 +8406,23 @@
         <v>160</v>
       </c>
       <c r="N24">
-        <f>COUNTIFS($G:$G,$M24,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f>COUNTIFS($G:$G,$M24,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P24">
-        <f>COUNTIFS($G:$G,$M24,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>COUNTIFS($G:$G,$M24,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R24">
-        <f>COUNTIFS($G:$G,$M24,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8332,23 +8458,23 @@
         <v>67</v>
       </c>
       <c r="N25">
-        <f>COUNTIFS($G:$G,$M25,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O25">
-        <f>COUNTIFS($G:$G,$M25,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P25">
-        <f>COUNTIFS($G:$G,$M25,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f>COUNTIFS($G:$G,$M25,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R25">
-        <f>COUNTIFS($G:$G,$M25,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8384,23 +8510,23 @@
         <v>10</v>
       </c>
       <c r="N26">
-        <f>COUNTIFS($G:$G,$M26,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O26">
-        <f>COUNTIFS($G:$G,$M26,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P26">
-        <f>COUNTIFS($G:$G,$M26,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f>COUNTIFS($G:$G,$M26,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R26">
-        <f>COUNTIFS($G:$G,$M26,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8436,23 +8562,23 @@
         <v>110</v>
       </c>
       <c r="N27">
-        <f>COUNTIFS($G:$G,$M27,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O27">
-        <f>COUNTIFS($G:$G,$M27,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P27">
-        <f>COUNTIFS($G:$G,$M27,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q27">
-        <f>COUNTIFS($G:$G,$M27,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R27">
-        <f>COUNTIFS($G:$G,$M27,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8488,23 +8614,23 @@
         <v>161</v>
       </c>
       <c r="N28">
-        <f>COUNTIFS($G:$G,$M28,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O28">
-        <f>COUNTIFS($G:$G,$M28,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P28">
-        <f>COUNTIFS($G:$G,$M28,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q28">
-        <f>COUNTIFS($G:$G,$M28,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R28">
-        <f>COUNTIFS($G:$G,$M28,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8540,23 +8666,23 @@
         <v>60</v>
       </c>
       <c r="N29">
-        <f>COUNTIFS($G:$G,$M29,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O29">
-        <f>COUNTIFS($G:$G,$M29,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P29">
-        <f>COUNTIFS($G:$G,$M29,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q29">
-        <f>COUNTIFS($G:$G,$M29,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="R29">
-        <f>COUNTIFS($G:$G,$M29,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8592,23 +8718,23 @@
         <v>162</v>
       </c>
       <c r="N30">
-        <f>COUNTIFS($G:$G,$M30,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O30">
-        <f>COUNTIFS($G:$G,$M30,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P30">
-        <f>COUNTIFS($G:$G,$M30,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f>COUNTIFS($G:$G,$M30,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R30">
-        <f>COUNTIFS($G:$G,$M30,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8644,23 +8770,23 @@
         <v>134</v>
       </c>
       <c r="N31">
-        <f>COUNTIFS($G:$G,$M31,$B:$B,N$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O31">
-        <f>COUNTIFS($G:$G,$M31,$B:$B,O$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P31">
-        <f>COUNTIFS($G:$G,$M31,$B:$B,P$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q31">
-        <f>COUNTIFS($G:$G,$M31,$B:$B,Q$1)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="R31">
-        <f>COUNTIFS($G:$G,$M31,$B:$B,R$1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -8696,23 +8822,23 @@
         <v>163</v>
       </c>
       <c r="N32">
-        <f>COUNTIFS($G:$G,$M32,$B:$B,N$1)</f>
+        <f t="shared" ref="N32:R41" si="5">COUNTIFS($G:$G,$M32,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O32">
-        <f>COUNTIFS($G:$G,$M32,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P32">
-        <f>COUNTIFS($G:$G,$M32,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q32">
-        <f>COUNTIFS($G:$G,$M32,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R32">
-        <f>COUNTIFS($G:$G,$M32,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8748,23 +8874,23 @@
         <v>164</v>
       </c>
       <c r="N33">
-        <f>COUNTIFS($G:$G,$M33,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O33">
-        <f>COUNTIFS($G:$G,$M33,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P33">
-        <f>COUNTIFS($G:$G,$M33,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f>COUNTIFS($G:$G,$M33,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R33">
-        <f>COUNTIFS($G:$G,$M33,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8800,23 +8926,23 @@
         <v>50</v>
       </c>
       <c r="N34">
-        <f>COUNTIFS($G:$G,$M34,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O34">
-        <f>COUNTIFS($G:$G,$M34,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P34">
-        <f>COUNTIFS($G:$G,$M34,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q34">
-        <f>COUNTIFS($G:$G,$M34,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R34">
-        <f>COUNTIFS($G:$G,$M34,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8852,23 +8978,23 @@
         <v>26</v>
       </c>
       <c r="N35">
-        <f>COUNTIFS($G:$G,$M35,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O35">
-        <f>COUNTIFS($G:$G,$M35,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f>COUNTIFS($G:$G,$M35,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q35">
-        <f>COUNTIFS($G:$G,$M35,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R35">
-        <f>COUNTIFS($G:$G,$M35,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8904,23 +9030,23 @@
         <v>87</v>
       </c>
       <c r="N36">
-        <f>COUNTIFS($G:$G,$M36,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O36">
-        <f>COUNTIFS($G:$G,$M36,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P36">
-        <f>COUNTIFS($G:$G,$M36,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q36">
-        <f>COUNTIFS($G:$G,$M36,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R36">
-        <f>COUNTIFS($G:$G,$M36,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -8956,23 +9082,23 @@
         <v>58</v>
       </c>
       <c r="N37">
-        <f>COUNTIFS($G:$G,$M37,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O37">
-        <f>COUNTIFS($G:$G,$M37,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P37">
-        <f>COUNTIFS($G:$G,$M37,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q37">
-        <f>COUNTIFS($G:$G,$M37,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="R37">
-        <f>COUNTIFS($G:$G,$M37,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9003,23 +9129,23 @@
         <v>97</v>
       </c>
       <c r="N38">
-        <f>COUNTIFS($G:$G,$M38,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O38">
-        <f>COUNTIFS($G:$G,$M38,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P38">
-        <f>COUNTIFS($G:$G,$M38,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q38">
-        <f>COUNTIFS($G:$G,$M38,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R38">
-        <f>COUNTIFS($G:$G,$M38,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9050,23 +9176,23 @@
         <v>165</v>
       </c>
       <c r="N39">
-        <f>COUNTIFS($G:$G,$M39,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O39">
-        <f>COUNTIFS($G:$G,$M39,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P39">
-        <f>COUNTIFS($G:$G,$M39,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q39">
-        <f>COUNTIFS($G:$G,$M39,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R39">
-        <f>COUNTIFS($G:$G,$M39,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9097,23 +9223,23 @@
         <v>143</v>
       </c>
       <c r="N40">
-        <f>COUNTIFS($G:$G,$M40,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O40">
-        <f>COUNTIFS($G:$G,$M40,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P40">
-        <f>COUNTIFS($G:$G,$M40,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q40">
-        <f>COUNTIFS($G:$G,$M40,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R40">
-        <f>COUNTIFS($G:$G,$M40,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9144,23 +9270,23 @@
         <v>52</v>
       </c>
       <c r="N41">
-        <f>COUNTIFS($G:$G,$M41,$B:$B,N$1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O41">
-        <f>COUNTIFS($G:$G,$M41,$B:$B,O$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P41">
-        <f>COUNTIFS($G:$G,$M41,$B:$B,P$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q41">
-        <f>COUNTIFS($G:$G,$M41,$B:$B,Q$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R41">
-        <f>COUNTIFS($G:$G,$M41,$B:$B,R$1)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -9191,23 +9317,23 @@
         <v>17</v>
       </c>
       <c r="N42">
-        <f>COUNTIFS($G:$G,$M42,$B:$B,N$1)</f>
+        <f t="shared" ref="N42:R51" si="6">COUNTIFS($G:$G,$M42,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O42">
-        <f>COUNTIFS($G:$G,$M42,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P42">
-        <f>COUNTIFS($G:$G,$M42,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q42">
-        <f>COUNTIFS($G:$G,$M42,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R42">
-        <f>COUNTIFS($G:$G,$M42,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -9238,23 +9364,23 @@
         <v>130</v>
       </c>
       <c r="N43">
-        <f>COUNTIFS($G:$G,$M43,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O43">
-        <f>COUNTIFS($G:$G,$M43,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P43">
-        <f>COUNTIFS($G:$G,$M43,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q43">
-        <f>COUNTIFS($G:$G,$M43,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R43">
-        <f>COUNTIFS($G:$G,$M43,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9285,23 +9411,23 @@
         <v>40</v>
       </c>
       <c r="N44">
-        <f>COUNTIFS($G:$G,$M44,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="O44">
-        <f>COUNTIFS($G:$G,$M44,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P44">
-        <f>COUNTIFS($G:$G,$M44,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q44">
-        <f>COUNTIFS($G:$G,$M44,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R44">
-        <f>COUNTIFS($G:$G,$M44,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9332,23 +9458,23 @@
         <v>94</v>
       </c>
       <c r="N45">
-        <f>COUNTIFS($G:$G,$M45,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O45">
-        <f>COUNTIFS($G:$G,$M45,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P45">
-        <f>COUNTIFS($G:$G,$M45,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q45">
-        <f>COUNTIFS($G:$G,$M45,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="R45">
-        <f>COUNTIFS($G:$G,$M45,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9379,23 +9505,23 @@
         <v>42</v>
       </c>
       <c r="N46">
-        <f>COUNTIFS($G:$G,$M46,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O46">
-        <f>COUNTIFS($G:$G,$M46,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P46">
-        <f>COUNTIFS($G:$G,$M46,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q46">
-        <f>COUNTIFS($G:$G,$M46,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R46">
-        <f>COUNTIFS($G:$G,$M46,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9426,23 +9552,23 @@
         <v>166</v>
       </c>
       <c r="N47">
-        <f>COUNTIFS($G:$G,$M47,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O47">
-        <f>COUNTIFS($G:$G,$M47,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P47">
-        <f>COUNTIFS($G:$G,$M47,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q47">
-        <f>COUNTIFS($G:$G,$M47,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R47">
-        <f>COUNTIFS($G:$G,$M47,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9473,23 +9599,23 @@
         <v>45</v>
       </c>
       <c r="N48">
-        <f>COUNTIFS($G:$G,$M48,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O48">
-        <f>COUNTIFS($G:$G,$M48,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P48">
-        <f>COUNTIFS($G:$G,$M48,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q48">
-        <f>COUNTIFS($G:$G,$M48,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="R48">
-        <f>COUNTIFS($G:$G,$M48,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9520,23 +9646,23 @@
         <v>167</v>
       </c>
       <c r="N49">
-        <f>COUNTIFS($G:$G,$M49,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O49">
-        <f>COUNTIFS($G:$G,$M49,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P49">
-        <f>COUNTIFS($G:$G,$M49,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q49">
-        <f>COUNTIFS($G:$G,$M49,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R49">
-        <f>COUNTIFS($G:$G,$M49,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9567,23 +9693,23 @@
         <v>24</v>
       </c>
       <c r="N50">
-        <f>COUNTIFS($G:$G,$M50,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O50">
-        <f>COUNTIFS($G:$G,$M50,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f>COUNTIFS($G:$G,$M50,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="Q50">
-        <f>COUNTIFS($G:$G,$M50,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R50">
-        <f>COUNTIFS($G:$G,$M50,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9612,23 +9738,23 @@
         <v>84</v>
       </c>
       <c r="N51">
-        <f>COUNTIFS($G:$G,$M51,$B:$B,N$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O51">
-        <f>COUNTIFS($G:$G,$M51,$B:$B,O$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P51">
-        <f>COUNTIFS($G:$G,$M51,$B:$B,P$1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q51">
-        <f>COUNTIFS($G:$G,$M51,$B:$B,Q$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R51">
-        <f>COUNTIFS($G:$G,$M51,$B:$B,R$1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9657,23 +9783,23 @@
         <v>99</v>
       </c>
       <c r="N52">
-        <f>COUNTIFS($G:$G,$M52,$B:$B,N$1)</f>
+        <f t="shared" ref="N52:R67" si="7">COUNTIFS($G:$G,$M52,$B:$B,N$1)</f>
         <v>0</v>
       </c>
       <c r="O52">
-        <f>COUNTIFS($G:$G,$M52,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P52">
-        <f>COUNTIFS($G:$G,$M52,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q52">
-        <f>COUNTIFS($G:$G,$M52,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="R52">
-        <f>COUNTIFS($G:$G,$M52,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9702,23 +9828,23 @@
         <v>55</v>
       </c>
       <c r="N53">
-        <f>COUNTIFS($G:$G,$M53,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O53">
-        <f>COUNTIFS($G:$G,$M53,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P53">
-        <f>COUNTIFS($G:$G,$M53,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q53">
-        <f>COUNTIFS($G:$G,$M53,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R53">
-        <f>COUNTIFS($G:$G,$M53,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9747,23 +9873,23 @@
         <v>32</v>
       </c>
       <c r="N54">
-        <f>COUNTIFS($G:$G,$M54,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O54">
-        <f>COUNTIFS($G:$G,$M54,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P54">
-        <f>COUNTIFS($G:$G,$M54,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q54">
-        <f>COUNTIFS($G:$G,$M54,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="R54">
-        <f>COUNTIFS($G:$G,$M54,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9792,23 +9918,23 @@
         <v>14</v>
       </c>
       <c r="N55">
-        <f>COUNTIFS($G:$G,$M55,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O55">
-        <f>COUNTIFS($G:$G,$M55,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P55">
-        <f>COUNTIFS($G:$G,$M55,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q55">
-        <f>COUNTIFS($G:$G,$M55,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R55">
-        <f>COUNTIFS($G:$G,$M55,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -9837,23 +9963,23 @@
         <v>168</v>
       </c>
       <c r="N56">
-        <f>COUNTIFS($G:$G,$M56,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O56">
-        <f>COUNTIFS($G:$G,$M56,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P56">
-        <f>COUNTIFS($G:$G,$M56,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q56">
-        <f>COUNTIFS($G:$G,$M56,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R56">
-        <f>COUNTIFS($G:$G,$M56,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9882,23 +10008,23 @@
         <v>169</v>
       </c>
       <c r="N57">
-        <f>COUNTIFS($G:$G,$M57,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O57">
-        <f>COUNTIFS($G:$G,$M57,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P57">
-        <f>COUNTIFS($G:$G,$M57,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q57">
-        <f>COUNTIFS($G:$G,$M57,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R57">
-        <f>COUNTIFS($G:$G,$M57,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9927,23 +10053,23 @@
         <v>170</v>
       </c>
       <c r="N58">
-        <f>COUNTIFS($G:$G,$M58,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O58">
-        <f>COUNTIFS($G:$G,$M58,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P58">
-        <f>COUNTIFS($G:$G,$M58,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q58">
-        <f>COUNTIFS($G:$G,$M58,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R58">
-        <f>COUNTIFS($G:$G,$M58,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -9972,23 +10098,23 @@
         <v>35</v>
       </c>
       <c r="N59">
-        <f>COUNTIFS($G:$G,$M59,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O59">
-        <f>COUNTIFS($G:$G,$M59,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P59">
-        <f>COUNTIFS($G:$G,$M59,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q59">
-        <f>COUNTIFS($G:$G,$M59,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="R59">
-        <f>COUNTIFS($G:$G,$M59,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10017,23 +10143,23 @@
         <v>38</v>
       </c>
       <c r="N60">
-        <f>COUNTIFS($G:$G,$M60,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O60">
-        <f>COUNTIFS($G:$G,$M60,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P60">
-        <f>COUNTIFS($G:$G,$M60,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q60">
-        <f>COUNTIFS($G:$G,$M60,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R60">
-        <f>COUNTIFS($G:$G,$M60,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10062,23 +10188,23 @@
         <v>62</v>
       </c>
       <c r="N61">
-        <f>COUNTIFS($G:$G,$M61,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O61">
-        <f>COUNTIFS($G:$G,$M61,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P61">
-        <f>COUNTIFS($G:$G,$M61,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q61">
-        <f>COUNTIFS($G:$G,$M61,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R61">
-        <f>COUNTIFS($G:$G,$M61,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10107,23 +10233,23 @@
         <v>28</v>
       </c>
       <c r="N62">
-        <f>COUNTIFS($G:$G,$M62,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="O62">
-        <f>COUNTIFS($G:$G,$M62,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P62">
-        <f>COUNTIFS($G:$G,$M62,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q62">
-        <f>COUNTIFS($G:$G,$M62,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R62">
-        <f>COUNTIFS($G:$G,$M62,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10152,23 +10278,23 @@
         <v>70</v>
       </c>
       <c r="N63">
-        <f>COUNTIFS($G:$G,$M63,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O63">
-        <f>COUNTIFS($G:$G,$M63,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="P63">
-        <f>COUNTIFS($G:$G,$M63,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q63">
-        <f>COUNTIFS($G:$G,$M63,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R63">
-        <f>COUNTIFS($G:$G,$M63,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10197,23 +10323,23 @@
         <v>22</v>
       </c>
       <c r="N64">
-        <f>COUNTIFS($G:$G,$M64,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="O64">
-        <f>COUNTIFS($G:$G,$M64,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P64">
-        <f>COUNTIFS($G:$G,$M64,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q64">
-        <f>COUNTIFS($G:$G,$M64,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R64">
-        <f>COUNTIFS($G:$G,$M64,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -10242,23 +10368,23 @@
         <v>12</v>
       </c>
       <c r="N65">
-        <f>COUNTIFS($G:$G,$M65,$B:$B,N$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="O65">
-        <f>COUNTIFS($G:$G,$M65,$B:$B,O$1)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P65">
-        <f>COUNTIFS($G:$G,$M65,$B:$B,P$1)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q65">
-        <f>COUNTIFS($G:$G,$M65,$B:$B,Q$1)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="R65">
-        <f>COUNTIFS($G:$G,$M65,$B:$B,R$1)</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
@@ -10283,6 +10409,29 @@
       <c r="I66" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="M66" t="s">
+        <v>136</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -10305,6 +10454,29 @@
       <c r="I67" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="M67" t="s">
+        <v>112</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -10327,6 +10499,29 @@
       <c r="I68" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="M68" t="s">
+        <v>227</v>
+      </c>
+      <c r="N68">
+        <f t="shared" ref="N68:R69" si="8">COUNTIFS($G:$G,$M68,$B:$B,N$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -10348,6 +10543,29 @@
       </c>
       <c r="I69" s="1" t="s">
         <v>213</v>
+      </c>
+      <c r="M69" t="s">
+        <v>228</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>